<commit_message>
Adding support for a more powerful tag format + a bug fix + documentation
</commit_message>
<xml_diff>
--- a/XLSInterview/exampleInterview.xlsx
+++ b/XLSInterview/exampleInterview.xlsx
@@ -4,74 +4,93 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="25575" windowHeight="12975"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="25575" windowHeight="12975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="interview" sheetId="1" r:id="rId1"/>
-    <sheet name="links" sheetId="5" r:id="rId2"/>
+    <sheet name="tags" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>What tasks do you find the most challenging or time consuming?</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>begin branch</t>
+  </si>
+  <si>
+    <t>end branch</t>
+  </si>
+  <si>
+    <t>Follow-on question</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>label</t>
+    <t>start</t>
+  </si>
+  <si>
+    <t>Subject does not do any computer related tasks.</t>
+  </si>
+  <si>
+    <t>Tell me about some of the tasks you use computers for?</t>
+  </si>
+  <si>
+    <t>imagePath</t>
+  </si>
+  <si>
+    <t>important</t>
+  </si>
+  <si>
+    <t>tangential</t>
+  </si>
+  <si>
+    <t>star.png</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
   <si>
     <t>tags</t>
   </si>
   <si>
-    <t>Tell me about some of the task your use computers for?</t>
-  </si>
-  <si>
-    <t>What tasks do you find the most challenging or time consuming?</t>
-  </si>
-  <si>
-    <t>Does not use computers.</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>computer_tasks</t>
-  </si>
-  <si>
-    <t>important, research further</t>
-  </si>
-  <si>
-    <t>noNextLink</t>
-  </si>
-  <si>
-    <t>computer_tasks_followup</t>
-  </si>
-  <si>
-    <t>Follow-up</t>
-  </si>
-  <si>
-    <t>interviewEnd</t>
-  </si>
-  <si>
-    <t>json/computer_tasks_followup</t>
+    <t>What was your first experience with a computer?</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>task_tags</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>data entry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -103,12 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -412,56 +430,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
+    </row>
+    <row r="7" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -471,50 +513,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>